<commit_message>
Added jira id in excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WATIAM.xlsx
+++ b/src/test/resources/xls/WATIAM.xlsx
@@ -34,13 +34,13 @@
     <t>Y</t>
   </si>
   <si>
-    <t>OPQA-TBD</t>
-  </si>
-  <si>
-    <t>Verify that user is able to login WoS Author Transformation Application using valid WAT Entitled account</t>
-  </si>
-  <si>
     <t>WATIAM001</t>
+  </si>
+  <si>
+    <t>WAT-231</t>
+  </si>
+  <si>
+    <t>Verify that Sign in using email and password (Steam Login)has been added to that login page</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -450,13 +450,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Developed new scripts in WATIAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WATIAM.xlsx
+++ b/src/test/resources/xls/WATIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>TCID</t>
   </si>
@@ -41,6 +41,60 @@
   </si>
   <si>
     <t>Verify that Sign in using email and password (Steam Login)has been added to that login page</t>
+  </si>
+  <si>
+    <t>WATIAM002</t>
+  </si>
+  <si>
+    <t>WAT-226</t>
+  </si>
+  <si>
+    <t>Verify that the app name is displayed as SaR Labs</t>
+  </si>
+  <si>
+    <t>WAT-227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the contact email is display as " sarlabs.info@clarivate.com " </t>
+  </si>
+  <si>
+    <t>WATIAM003</t>
+  </si>
+  <si>
+    <t>WATIAM004</t>
+  </si>
+  <si>
+    <t>WAT-228</t>
+  </si>
+  <si>
+    <t>Verify that the marketing text module should not appear in the login page</t>
+  </si>
+  <si>
+    <t>WATIAM005</t>
+  </si>
+  <si>
+    <t>WAT-229</t>
+  </si>
+  <si>
+    <t>Verify that the links to the Terms and Privacy Statement should appear in login page</t>
+  </si>
+  <si>
+    <t>WATIAM006</t>
+  </si>
+  <si>
+    <t>Verify that Link to forgot password should be available on the sign in page</t>
+  </si>
+  <si>
+    <t>WAT-232</t>
+  </si>
+  <si>
+    <t>WATIAM007</t>
+  </si>
+  <si>
+    <t>Verify that standard platform auth error messaging is displayed when Email address is not properly formatted</t>
+  </si>
+  <si>
+    <t>WAT-235</t>
   </si>
 </sst>
 </file>
@@ -416,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -463,6 +517,96 @@
       </c>
       <c r="E2" s="4"/>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created new scripts in WATIAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WATIAM.xlsx
+++ b/src/test/resources/xls/WATIAM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>TCID</t>
   </si>
@@ -95,6 +95,42 @@
   </si>
   <si>
     <t>WAT-235</t>
+  </si>
+  <si>
+    <t>WATIAM008</t>
+  </si>
+  <si>
+    <t>WAT-238</t>
+  </si>
+  <si>
+    <t>Verify that standard platform auth error messaging is displayed when Email/password combination are not found in STeAM</t>
+  </si>
+  <si>
+    <t>WATIAM009</t>
+  </si>
+  <si>
+    <t>WAT-239&amp;WAT-240</t>
+  </si>
+  <si>
+    <t>Verify that standard platform auth error messaging is displayed when Email field is left blank and submit button is clicked&amp;Verify that standard platform auth error messaging is displayed when password field is left blank and submit button is clicked</t>
+  </si>
+  <si>
+    <t>WATIAM010</t>
+  </si>
+  <si>
+    <t>WAT-241&amp;WAT-242</t>
+  </si>
+  <si>
+    <t>Verify that the system shall lock a user after TBD failed attempts to sign in with an incorrect email or password combination&amp;Verify that the system shall prevent a locked user from accessing the WAT app and message when account is locked using standard auth error messaging</t>
+  </si>
+  <si>
+    <t>WATIAM011</t>
+  </si>
+  <si>
+    <t>Verify that the system shall prevent an evicted user from accessing the WAT app and message when account is suspended using standard auth error messaging</t>
+  </si>
+  <si>
+    <t>WAT-243</t>
   </si>
 </sst>
 </file>
@@ -470,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -607,6 +643,66 @@
       </c>
       <c r="E8" s="4"/>
     </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="28.8">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="43.2">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.8">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New Script added in WATIAM Module.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/WATIAM.xlsx
+++ b/src/test/resources/xls/WATIAM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>TCID</t>
   </si>
@@ -131,6 +131,16 @@
   </si>
   <si>
     <t>WAT-243</t>
+  </si>
+  <si>
+    <t>WATIAM012</t>
+  </si>
+  <si>
+    <t>WAT-252||WAT-253||WAT-559||WAT-254||WAT-255||WAT-256||WAT-257||WAT-258||
+WAT-281||WAT-282||WAT-259||WAT-560||WAT-260||WAT-261||WAT-262||WAT-263||WAT-264||WAT-265||WAT-266||WAT-267||WAT-268||WAT-269||WAT-270||WAT-271||WAT-272||WAT-273||WAT-274||WAT-275</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on WAT Landing page||Verify that Thomson Reuters is replaced with Clarivate Analytics to all WAT pages related forgot password&amp;&amp;Verify that Thomson Reuters logo is replaced with Clarivate Analytics logo.||Verify that 'SaR Labs' should be moved within the white area (above and centered over the 'Forgot Password' text).||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a WAT password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that The support contact email in the email body is sarlabs@clarivate.com||Verify that The support contact email in the footer is sarlabs@clarivate.com||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that 'SaR Labs' should be moved within the white area||Verify Password must have at least one special character from !@#$%^*()~`{}[]| in reset password page||Verify Password must contain at least one number is ALWAYS enforced in password reset page||Verify Password must have at least one alphabet character either upper or lower case is ALWAYS enforced in reset password page.||Verify Password Maximum Length of 95 characters is ALWAYS enforced in reset password page.||Verify that External Password Reset Page should have a new password field where the user enters their new password.&amp;&amp; Verify that the Password minimum length of 8 characters is ALWAYS enforced in reset password page.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format||Verify that error message New password should not match current password. when enter Old and New password are same in reset password page.||Verify that error message New password should not match previous 4 passwords. when enter new password match with previous four passwords in reset password page.</t>
   </si>
 </sst>
 </file>
@@ -506,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -703,6 +713,21 @@
       </c>
       <c r="E12" s="4"/>
     </row>
+    <row r="13" spans="1:5" ht="144">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>